<commit_message>
cambios de layout y acumulados para anahi
</commit_message>
<xml_diff>
--- a/OperadoraNominas/bin/Debug/Archivos/timbrado_ademsa_q.xlsx
+++ b/OperadoraNominas/bin/Debug/Archivos/timbrado_ademsa_q.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.1.225\nominas\VIGENTES\ADEMSA\QUINCENAL\4. TIMBRADO\2Q FEBRERO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollo\TMMSQ\OperadoraNominas\OperadoraNominas\bin\Debug\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Generales" sheetId="2" r:id="rId1"/>
@@ -60,7 +60,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="Q1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -104,7 +104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="R1" authorId="0" shapeId="0">
+    <comment ref="S1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -129,7 +129,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="V1" authorId="0" shapeId="0">
+    <comment ref="W1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -147,7 +147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="X1" authorId="0" shapeId="0">
+    <comment ref="Y1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z1" authorId="0" shapeId="0">
+    <comment ref="AA1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -259,7 +259,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1054" uniqueCount="424">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="425">
   <si>
     <t>No. Empleado</t>
   </si>
@@ -1531,6 +1531,9 @@
   </si>
   <si>
     <t>=S4-T4</t>
+  </si>
+  <si>
+    <t>Código P.</t>
   </si>
 </sst>
 </file>
@@ -1954,7 +1957,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -2028,6 +2031,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -2333,13 +2337,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AC41"/>
+  <dimension ref="A1:AD41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="P14" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="3" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C20" sqref="C20"/>
+      <selection pane="bottomRight" activeCell="K1" sqref="K1:K1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,25 +2357,26 @@
     <col min="7" max="8" width="9.7109375" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="14.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
-    <col min="12" max="12" width="20.7109375" customWidth="1"/>
-    <col min="13" max="14" width="9.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.7109375" customWidth="1"/>
-    <col min="16" max="16" width="5.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="6.7109375" customWidth="1"/>
-    <col min="19" max="19" width="15.7109375" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" customWidth="1"/>
-    <col min="21" max="21" width="29.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="25" width="9.7109375" customWidth="1"/>
-    <col min="26" max="26" width="5.7109375" customWidth="1"/>
-    <col min="27" max="27" width="19.7109375" customWidth="1"/>
-    <col min="28" max="28" width="16.7109375" customWidth="1"/>
-    <col min="29" max="29" width="35.85546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="31" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="14.7109375" style="20" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" customWidth="1"/>
+    <col min="13" max="13" width="20.7109375" customWidth="1"/>
+    <col min="14" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" customWidth="1"/>
+    <col min="17" max="17" width="5.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="6.7109375" customWidth="1"/>
+    <col min="20" max="20" width="15.7109375" customWidth="1"/>
+    <col min="21" max="21" width="17.7109375" customWidth="1"/>
+    <col min="22" max="22" width="29.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="9.7109375" customWidth="1"/>
+    <col min="27" max="27" width="5.7109375" customWidth="1"/>
+    <col min="28" max="28" width="19.7109375" customWidth="1"/>
+    <col min="29" max="29" width="16.7109375" customWidth="1"/>
+    <col min="30" max="30" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="32" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2403,52 +2408,55 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="N1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="37"/>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="37"/>
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="36" t="s">
+      <c r="Q1" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="37"/>
-      <c r="R1" s="36" t="s">
+      <c r="R1" s="37"/>
+      <c r="S1" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="S1" s="37"/>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="37"/>
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="W1" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="37"/>
-      <c r="X1" s="36" t="s">
+      <c r="X1" s="37"/>
+      <c r="Y1" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="36" t="s">
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="1" t="s">
+      <c r="AB1" s="37"/>
+      <c r="AC1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
         <v>100</v>
       </c>
@@ -2479,54 +2487,55 @@
       <c r="J2" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K2" s="23">
+      <c r="K2" s="47"/>
+      <c r="L2" s="23">
         <v>15</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="M2" s="23" t="s">
         <v>338</v>
       </c>
-      <c r="M2" s="20">
+      <c r="N2" s="20">
         <v>1</v>
       </c>
-      <c r="N2" s="20" t="s">
+      <c r="O2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="20">
+      <c r="Q2" s="20">
         <v>1</v>
       </c>
-      <c r="Q2" s="20" t="s">
+      <c r="R2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="20">
+      <c r="S2" s="20">
         <v>2</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="T2" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T2" s="23" t="s">
+      <c r="U2" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="U2" s="23" t="s">
+      <c r="V2" s="23" t="s">
         <v>375</v>
       </c>
-      <c r="V2" s="20">
+      <c r="W2" s="20">
         <v>4</v>
       </c>
-      <c r="W2" s="20" t="s">
+      <c r="X2" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X2" s="20">
+      <c r="Y2" s="20">
         <v>2</v>
       </c>
-      <c r="Y2" s="20" t="s">
+      <c r="Z2" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="AA2" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC2" s="27"/>
-    </row>
-    <row r="3" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD2" s="27"/>
+    </row>
+    <row r="3" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="23" t="s">
         <v>106</v>
       </c>
@@ -2557,54 +2566,55 @@
       <c r="J3" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="25"/>
+      <c r="L3" s="23">
         <v>15</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="M3" s="23" t="s">
         <v>339</v>
       </c>
-      <c r="M3" s="20">
+      <c r="N3" s="20">
         <v>1</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="O3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="20">
+      <c r="Q3" s="20">
         <v>1</v>
       </c>
-      <c r="Q3" s="20" t="s">
+      <c r="R3" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="20">
+      <c r="S3" s="20">
         <v>2</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="T3" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T3" s="23" t="s">
+      <c r="U3" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="U3" s="23" t="s">
+      <c r="V3" s="23" t="s">
         <v>377</v>
       </c>
-      <c r="V3" s="20">
+      <c r="W3" s="20">
         <v>4</v>
       </c>
-      <c r="W3" s="20" t="s">
+      <c r="X3" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X3" s="20">
+      <c r="Y3" s="20">
         <v>2</v>
       </c>
-      <c r="Y3" s="20" t="s">
+      <c r="Z3" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z3" s="23" t="s">
+      <c r="AA3" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC3" s="27"/>
-    </row>
-    <row r="4" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD3" s="27"/>
+    </row>
+    <row r="4" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="23" t="s">
         <v>112</v>
       </c>
@@ -2635,54 +2645,55 @@
       <c r="J4" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="25"/>
+      <c r="L4" s="23">
         <v>15</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="M4" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="M4" s="20">
+      <c r="N4" s="20">
         <v>1</v>
       </c>
-      <c r="N4" s="20" t="s">
+      <c r="O4" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P4" s="20">
+      <c r="Q4" s="20">
         <v>1</v>
       </c>
-      <c r="Q4" s="20" t="s">
+      <c r="R4" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R4" s="20">
+      <c r="S4" s="20">
         <v>2</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="T4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T4" s="23" t="s">
+      <c r="U4" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="U4" s="23" t="s">
+      <c r="V4" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="V4" s="20">
+      <c r="W4" s="20">
         <v>4</v>
       </c>
-      <c r="W4" s="20" t="s">
+      <c r="X4" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X4" s="20">
+      <c r="Y4" s="20">
         <v>2</v>
       </c>
-      <c r="Y4" s="20" t="s">
+      <c r="Z4" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z4" s="23" t="s">
+      <c r="AA4" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC4" s="27"/>
-    </row>
-    <row r="5" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD4" s="27"/>
+    </row>
+    <row r="5" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="23" t="s">
         <v>118</v>
       </c>
@@ -2713,54 +2724,55 @@
       <c r="J5" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="25"/>
+      <c r="L5" s="23">
         <v>15</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="M5" s="23" t="s">
         <v>341</v>
       </c>
-      <c r="M5" s="20">
+      <c r="N5" s="20">
         <v>1</v>
       </c>
-      <c r="N5" s="20" t="s">
+      <c r="O5" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P5" s="20">
+      <c r="Q5" s="20">
         <v>1</v>
       </c>
-      <c r="Q5" s="20" t="s">
+      <c r="R5" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R5" s="20">
+      <c r="S5" s="20">
         <v>2</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="T5" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T5" s="23" t="s">
+      <c r="U5" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="U5" s="23" t="s">
+      <c r="V5" s="23" t="s">
         <v>380</v>
       </c>
-      <c r="V5" s="20">
+      <c r="W5" s="20">
         <v>4</v>
       </c>
-      <c r="W5" s="20" t="s">
+      <c r="X5" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X5" s="20">
+      <c r="Y5" s="20">
         <v>2</v>
       </c>
-      <c r="Y5" s="20" t="s">
+      <c r="Z5" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="AA5" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC5" s="27"/>
-    </row>
-    <row r="6" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD5" s="27"/>
+    </row>
+    <row r="6" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="23" t="s">
         <v>124</v>
       </c>
@@ -2791,54 +2803,55 @@
       <c r="J6" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="25"/>
+      <c r="L6" s="23">
         <v>15</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="M6" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="M6" s="20">
+      <c r="N6" s="20">
         <v>1</v>
       </c>
-      <c r="N6" s="20" t="s">
+      <c r="O6" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P6" s="20">
+      <c r="Q6" s="20">
         <v>1</v>
       </c>
-      <c r="Q6" s="20" t="s">
+      <c r="R6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R6" s="20">
+      <c r="S6" s="20">
         <v>2</v>
       </c>
-      <c r="S6" s="20" t="s">
+      <c r="T6" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T6" s="23" t="s">
+      <c r="U6" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="U6" s="23" t="s">
+      <c r="V6" s="23" t="s">
         <v>382</v>
       </c>
-      <c r="V6" s="20">
+      <c r="W6" s="20">
         <v>4</v>
       </c>
-      <c r="W6" s="20" t="s">
+      <c r="X6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X6" s="20">
+      <c r="Y6" s="20">
         <v>2</v>
       </c>
-      <c r="Y6" s="20" t="s">
+      <c r="Z6" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z6" s="23" t="s">
+      <c r="AA6" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="AC6" s="27"/>
-    </row>
-    <row r="7" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD6" s="27"/>
+    </row>
+    <row r="7" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
         <v>130</v>
       </c>
@@ -2869,54 +2882,55 @@
       <c r="J7" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="25"/>
+      <c r="L7" s="23">
         <v>15</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="M7" s="23" t="s">
         <v>343</v>
       </c>
-      <c r="M7" s="20">
+      <c r="N7" s="20">
         <v>1</v>
       </c>
-      <c r="N7" s="20" t="s">
+      <c r="O7" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P7" s="20">
+      <c r="Q7" s="20">
         <v>1</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="R7" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R7" s="20">
+      <c r="S7" s="20">
         <v>2</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="T7" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="U7" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="U7" s="23" t="s">
+      <c r="V7" s="23" t="s">
         <v>383</v>
       </c>
-      <c r="V7" s="20">
+      <c r="W7" s="20">
         <v>4</v>
       </c>
-      <c r="W7" s="20" t="s">
+      <c r="X7" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X7" s="20">
+      <c r="Y7" s="20">
         <v>2</v>
       </c>
-      <c r="Y7" s="20" t="s">
+      <c r="Z7" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z7" s="23" t="s">
+      <c r="AA7" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="AC7" s="27"/>
-    </row>
-    <row r="8" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD7" s="27"/>
+    </row>
+    <row r="8" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>136</v>
       </c>
@@ -2947,54 +2961,55 @@
       <c r="J8" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="25"/>
+      <c r="L8" s="23">
         <v>15</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="M8" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="M8" s="20">
+      <c r="N8" s="20">
         <v>1</v>
       </c>
-      <c r="N8" s="20" t="s">
+      <c r="O8" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P8" s="20">
+      <c r="Q8" s="20">
         <v>1</v>
       </c>
-      <c r="Q8" s="20" t="s">
+      <c r="R8" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R8" s="20">
+      <c r="S8" s="20">
         <v>2</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="T8" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T8" s="23" t="s">
+      <c r="U8" s="23" t="s">
         <v>384</v>
       </c>
-      <c r="U8" s="23" t="s">
+      <c r="V8" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="V8" s="20">
+      <c r="W8" s="20">
         <v>4</v>
       </c>
-      <c r="W8" s="20" t="s">
+      <c r="X8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X8" s="20">
+      <c r="Y8" s="20">
         <v>2</v>
       </c>
-      <c r="Y8" s="20" t="s">
+      <c r="Z8" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z8" s="23" t="s">
+      <c r="AA8" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC8" s="27"/>
-    </row>
-    <row r="9" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD8" s="27"/>
+    </row>
+    <row r="9" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
         <v>142</v>
       </c>
@@ -3025,54 +3040,55 @@
       <c r="J9" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="25"/>
+      <c r="L9" s="23">
         <v>15</v>
       </c>
-      <c r="L9" s="23" t="s">
+      <c r="M9" s="23" t="s">
         <v>345</v>
       </c>
-      <c r="M9" s="20">
+      <c r="N9" s="20">
         <v>1</v>
       </c>
-      <c r="N9" s="20" t="s">
+      <c r="O9" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P9" s="20">
+      <c r="Q9" s="20">
         <v>1</v>
       </c>
-      <c r="Q9" s="20" t="s">
+      <c r="R9" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R9" s="20">
+      <c r="S9" s="20">
         <v>2</v>
       </c>
-      <c r="S9" s="20" t="s">
+      <c r="T9" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T9" s="23" t="s">
+      <c r="U9" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="U9" s="23" t="s">
+      <c r="V9" s="23" t="s">
         <v>386</v>
       </c>
-      <c r="V9" s="20">
+      <c r="W9" s="20">
         <v>4</v>
       </c>
-      <c r="W9" s="20" t="s">
+      <c r="X9" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X9" s="20">
+      <c r="Y9" s="20">
         <v>2</v>
       </c>
-      <c r="Y9" s="20" t="s">
+      <c r="Z9" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z9" s="23" t="s">
+      <c r="AA9" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC9" s="27"/>
-    </row>
-    <row r="10" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD9" s="27"/>
+    </row>
+    <row r="10" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>148</v>
       </c>
@@ -3103,54 +3119,55 @@
       <c r="J10" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="23">
+      <c r="K10" s="25"/>
+      <c r="L10" s="23">
         <v>15</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="M10" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="M10" s="20">
+      <c r="N10" s="20">
         <v>1</v>
       </c>
-      <c r="N10" s="20" t="s">
+      <c r="O10" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="20">
+      <c r="Q10" s="20">
         <v>1</v>
       </c>
-      <c r="Q10" s="20" t="s">
+      <c r="R10" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="20">
+      <c r="S10" s="20">
         <v>2</v>
       </c>
-      <c r="S10" s="20" t="s">
+      <c r="T10" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T10" s="23" t="s">
+      <c r="U10" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="U10" s="23" t="s">
+      <c r="V10" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="V10" s="20">
+      <c r="W10" s="20">
         <v>4</v>
       </c>
-      <c r="W10" s="20" t="s">
+      <c r="X10" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X10" s="20">
+      <c r="Y10" s="20">
         <v>2</v>
       </c>
-      <c r="Y10" s="20" t="s">
+      <c r="Z10" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z10" s="23" t="s">
+      <c r="AA10" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC10" s="27"/>
-    </row>
-    <row r="11" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD10" s="27"/>
+    </row>
+    <row r="11" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="23" t="s">
         <v>154</v>
       </c>
@@ -3181,54 +3198,55 @@
       <c r="J11" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K11" s="23">
+      <c r="K11" s="25"/>
+      <c r="L11" s="23">
         <v>15</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="M11" s="23" t="s">
         <v>347</v>
       </c>
-      <c r="M11" s="20">
+      <c r="N11" s="20">
         <v>1</v>
       </c>
-      <c r="N11" s="20" t="s">
+      <c r="O11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P11" s="20">
+      <c r="Q11" s="20">
         <v>1</v>
       </c>
-      <c r="Q11" s="20" t="s">
+      <c r="R11" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R11" s="20">
+      <c r="S11" s="20">
         <v>2</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="T11" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T11" s="23" t="s">
+      <c r="U11" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U11" s="23" t="s">
+      <c r="V11" s="23" t="s">
         <v>390</v>
       </c>
-      <c r="V11" s="20">
+      <c r="W11" s="20">
         <v>4</v>
       </c>
-      <c r="W11" s="20" t="s">
+      <c r="X11" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X11" s="20">
+      <c r="Y11" s="20">
         <v>2</v>
       </c>
-      <c r="Y11" s="20" t="s">
+      <c r="Z11" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z11" s="23" t="s">
+      <c r="AA11" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC11" s="27"/>
-    </row>
-    <row r="12" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD11" s="27"/>
+    </row>
+    <row r="12" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="23" t="s">
         <v>160</v>
       </c>
@@ -3259,54 +3277,55 @@
       <c r="J12" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K12" s="23">
+      <c r="K12" s="25"/>
+      <c r="L12" s="23">
         <v>15</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="M12" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="M12" s="20">
+      <c r="N12" s="20">
         <v>1</v>
       </c>
-      <c r="N12" s="20" t="s">
+      <c r="O12" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="20">
+      <c r="Q12" s="20">
         <v>1</v>
       </c>
-      <c r="Q12" s="20" t="s">
+      <c r="R12" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R12" s="20">
+      <c r="S12" s="20">
         <v>2</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="T12" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T12" s="23" t="s">
+      <c r="U12" s="23" t="s">
         <v>378</v>
       </c>
-      <c r="U12" s="23" t="s">
+      <c r="V12" s="23" t="s">
         <v>391</v>
       </c>
-      <c r="V12" s="20">
+      <c r="W12" s="20">
         <v>4</v>
       </c>
-      <c r="W12" s="20" t="s">
+      <c r="X12" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X12" s="20">
+      <c r="Y12" s="20">
         <v>2</v>
       </c>
-      <c r="Y12" s="20" t="s">
+      <c r="Z12" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z12" s="23" t="s">
+      <c r="AA12" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC12" s="27"/>
-    </row>
-    <row r="13" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD12" s="27"/>
+    </row>
+    <row r="13" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>166</v>
       </c>
@@ -3337,54 +3356,55 @@
       <c r="J13" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K13" s="23">
+      <c r="K13" s="25"/>
+      <c r="L13" s="23">
         <v>15</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="M13" s="23" t="s">
         <v>349</v>
       </c>
-      <c r="M13" s="20">
+      <c r="N13" s="20">
         <v>1</v>
       </c>
-      <c r="N13" s="20" t="s">
+      <c r="O13" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P13" s="20">
+      <c r="Q13" s="20">
         <v>1</v>
       </c>
-      <c r="Q13" s="20" t="s">
+      <c r="R13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R13" s="20">
+      <c r="S13" s="20">
         <v>2</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="T13" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T13" s="23" t="s">
+      <c r="U13" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="U13" s="23" t="s">
+      <c r="V13" s="23" t="s">
         <v>392</v>
       </c>
-      <c r="V13" s="20">
+      <c r="W13" s="20">
         <v>4</v>
       </c>
-      <c r="W13" s="20" t="s">
+      <c r="X13" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X13" s="20">
+      <c r="Y13" s="20">
         <v>2</v>
       </c>
-      <c r="Y13" s="20" t="s">
+      <c r="Z13" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z13" s="23" t="s">
+      <c r="AA13" s="23" t="s">
         <v>418</v>
       </c>
-      <c r="AC13" s="27"/>
-    </row>
-    <row r="14" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD13" s="27"/>
+    </row>
+    <row r="14" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>172</v>
       </c>
@@ -3415,54 +3435,55 @@
       <c r="J14" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K14" s="23">
+      <c r="K14" s="25"/>
+      <c r="L14" s="23">
         <v>15</v>
       </c>
-      <c r="L14" s="23" t="s">
+      <c r="M14" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="M14" s="20">
+      <c r="N14" s="20">
         <v>1</v>
       </c>
-      <c r="N14" s="20" t="s">
+      <c r="O14" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P14" s="20">
+      <c r="Q14" s="20">
         <v>1</v>
       </c>
-      <c r="Q14" s="20" t="s">
+      <c r="R14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R14" s="20">
+      <c r="S14" s="20">
         <v>2</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="T14" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T14" s="23" t="s">
+      <c r="U14" s="23" t="s">
         <v>385</v>
       </c>
-      <c r="U14" s="23" t="s">
+      <c r="V14" s="23" t="s">
         <v>393</v>
       </c>
-      <c r="V14" s="20">
+      <c r="W14" s="20">
         <v>4</v>
       </c>
-      <c r="W14" s="20" t="s">
+      <c r="X14" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X14" s="20">
+      <c r="Y14" s="20">
         <v>2</v>
       </c>
-      <c r="Y14" s="20" t="s">
+      <c r="Z14" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z14" s="23" t="s">
+      <c r="AA14" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC14" s="27"/>
-    </row>
-    <row r="15" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD14" s="27"/>
+    </row>
+    <row r="15" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>178</v>
       </c>
@@ -3493,54 +3514,55 @@
       <c r="J15" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K15" s="23">
+      <c r="K15" s="25"/>
+      <c r="L15" s="23">
         <v>15</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="M15" s="23" t="s">
         <v>351</v>
       </c>
-      <c r="M15" s="20">
+      <c r="N15" s="20">
         <v>1</v>
       </c>
-      <c r="N15" s="20" t="s">
+      <c r="O15" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P15" s="20">
+      <c r="Q15" s="20">
         <v>1</v>
       </c>
-      <c r="Q15" s="20" t="s">
+      <c r="R15" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R15" s="20">
+      <c r="S15" s="20">
         <v>2</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="T15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T15" s="23" t="s">
+      <c r="U15" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="U15" s="23" t="s">
+      <c r="V15" s="23" t="s">
         <v>394</v>
       </c>
-      <c r="V15" s="20">
+      <c r="W15" s="20">
         <v>4</v>
       </c>
-      <c r="W15" s="20" t="s">
+      <c r="X15" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X15" s="20">
+      <c r="Y15" s="20">
         <v>2</v>
       </c>
-      <c r="Y15" s="20" t="s">
+      <c r="Z15" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z15" s="23" t="s">
+      <c r="AA15" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC15" s="27"/>
-    </row>
-    <row r="16" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD15" s="27"/>
+    </row>
+    <row r="16" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>184</v>
       </c>
@@ -3571,54 +3593,55 @@
       <c r="J16" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K16" s="23">
+      <c r="K16" s="25"/>
+      <c r="L16" s="23">
         <v>15</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="M16" s="23" t="s">
         <v>352</v>
       </c>
-      <c r="M16" s="20">
+      <c r="N16" s="20">
         <v>1</v>
       </c>
-      <c r="N16" s="20" t="s">
+      <c r="O16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P16" s="20">
+      <c r="Q16" s="20">
         <v>1</v>
       </c>
-      <c r="Q16" s="20" t="s">
+      <c r="R16" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R16" s="20">
+      <c r="S16" s="20">
         <v>2</v>
       </c>
-      <c r="S16" s="20" t="s">
+      <c r="T16" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T16" s="23" t="s">
+      <c r="U16" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="U16" s="23" t="s">
+      <c r="V16" s="23" t="s">
         <v>395</v>
       </c>
-      <c r="V16" s="20">
+      <c r="W16" s="20">
         <v>4</v>
       </c>
-      <c r="W16" s="20" t="s">
+      <c r="X16" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X16" s="20">
+      <c r="Y16" s="20">
         <v>2</v>
       </c>
-      <c r="Y16" s="20" t="s">
+      <c r="Z16" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z16" s="23" t="s">
+      <c r="AA16" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC16" s="27"/>
-    </row>
-    <row r="17" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD16" s="27"/>
+    </row>
+    <row r="17" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>190</v>
       </c>
@@ -3649,54 +3672,55 @@
       <c r="J17" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K17" s="23">
+      <c r="K17" s="25"/>
+      <c r="L17" s="23">
         <v>15</v>
       </c>
-      <c r="L17" s="23" t="s">
+      <c r="M17" s="23" t="s">
         <v>353</v>
       </c>
-      <c r="M17" s="20">
+      <c r="N17" s="20">
         <v>1</v>
       </c>
-      <c r="N17" s="20" t="s">
+      <c r="O17" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P17" s="20">
+      <c r="Q17" s="20">
         <v>1</v>
       </c>
-      <c r="Q17" s="20" t="s">
+      <c r="R17" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R17" s="20">
+      <c r="S17" s="20">
         <v>2</v>
       </c>
-      <c r="S17" s="20" t="s">
+      <c r="T17" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T17" s="23" t="s">
+      <c r="U17" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="U17" s="23" t="s">
+      <c r="V17" s="23" t="s">
         <v>396</v>
       </c>
-      <c r="V17" s="20">
+      <c r="W17" s="20">
         <v>4</v>
       </c>
-      <c r="W17" s="20" t="s">
+      <c r="X17" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X17" s="20">
+      <c r="Y17" s="20">
         <v>2</v>
       </c>
-      <c r="Y17" s="20" t="s">
+      <c r="Z17" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z17" s="23" t="s">
+      <c r="AA17" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="AC17" s="27"/>
-    </row>
-    <row r="18" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD17" s="27"/>
+    </row>
+    <row r="18" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>196</v>
       </c>
@@ -3727,54 +3751,55 @@
       <c r="J18" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K18" s="23">
+      <c r="K18" s="25"/>
+      <c r="L18" s="23">
         <v>15</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="M18" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="M18" s="20">
+      <c r="N18" s="20">
         <v>1</v>
       </c>
-      <c r="N18" s="20" t="s">
+      <c r="O18" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P18" s="20">
+      <c r="Q18" s="20">
         <v>1</v>
       </c>
-      <c r="Q18" s="20" t="s">
+      <c r="R18" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R18" s="20">
+      <c r="S18" s="20">
         <v>2</v>
       </c>
-      <c r="S18" s="20" t="s">
+      <c r="T18" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T18" s="23" t="s">
+      <c r="U18" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="U18" s="23" t="s">
+      <c r="V18" s="23" t="s">
         <v>397</v>
       </c>
-      <c r="V18" s="20">
+      <c r="W18" s="20">
         <v>4</v>
       </c>
-      <c r="W18" s="20" t="s">
+      <c r="X18" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X18" s="20">
+      <c r="Y18" s="20">
         <v>2</v>
       </c>
-      <c r="Y18" s="20" t="s">
+      <c r="Z18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z18" s="23" t="s">
+      <c r="AA18" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC18" s="27"/>
-    </row>
-    <row r="19" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD18" s="27"/>
+    </row>
+    <row r="19" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="23" t="s">
         <v>202</v>
       </c>
@@ -3805,54 +3830,55 @@
       <c r="J19" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="23">
+      <c r="K19" s="25"/>
+      <c r="L19" s="23">
         <v>15</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="M19" s="23" t="s">
         <v>355</v>
       </c>
-      <c r="M19" s="20">
+      <c r="N19" s="20">
         <v>1</v>
       </c>
-      <c r="N19" s="20" t="s">
+      <c r="O19" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P19" s="20">
+      <c r="Q19" s="20">
         <v>1</v>
       </c>
-      <c r="Q19" s="20" t="s">
+      <c r="R19" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R19" s="20">
+      <c r="S19" s="20">
         <v>2</v>
       </c>
-      <c r="S19" s="20" t="s">
+      <c r="T19" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T19" s="23" t="s">
+      <c r="U19" s="23" t="s">
         <v>398</v>
       </c>
-      <c r="U19" s="23" t="s">
+      <c r="V19" s="23" t="s">
         <v>399</v>
       </c>
-      <c r="V19" s="20">
+      <c r="W19" s="20">
         <v>4</v>
       </c>
-      <c r="W19" s="20" t="s">
+      <c r="X19" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X19" s="20">
+      <c r="Y19" s="20">
         <v>2</v>
       </c>
-      <c r="Y19" s="20" t="s">
+      <c r="Z19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z19" s="23" t="s">
+      <c r="AA19" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="AC19" s="27"/>
-    </row>
-    <row r="20" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD19" s="27"/>
+    </row>
+    <row r="20" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="23" t="s">
         <v>208</v>
       </c>
@@ -3883,54 +3909,55 @@
       <c r="J20" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K20" s="23">
+      <c r="K20" s="25"/>
+      <c r="L20" s="23">
         <v>15</v>
       </c>
-      <c r="L20" s="23" t="s">
+      <c r="M20" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="M20" s="20">
+      <c r="N20" s="20">
         <v>1</v>
       </c>
-      <c r="N20" s="20" t="s">
+      <c r="O20" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P20" s="20">
+      <c r="Q20" s="20">
         <v>1</v>
       </c>
-      <c r="Q20" s="20" t="s">
+      <c r="R20" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R20" s="20">
+      <c r="S20" s="20">
         <v>2</v>
       </c>
-      <c r="S20" s="20" t="s">
+      <c r="T20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T20" s="23" t="s">
+      <c r="U20" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="U20" s="23" t="s">
+      <c r="V20" s="23" t="s">
         <v>400</v>
       </c>
-      <c r="V20" s="20">
+      <c r="W20" s="20">
         <v>4</v>
       </c>
-      <c r="W20" s="20" t="s">
+      <c r="X20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X20" s="20">
+      <c r="Y20" s="20">
         <v>2</v>
       </c>
-      <c r="Y20" s="20" t="s">
+      <c r="Z20" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z20" s="23" t="s">
+      <c r="AA20" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC20" s="27"/>
-    </row>
-    <row r="21" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD20" s="27"/>
+    </row>
+    <row r="21" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="23" t="s">
         <v>214</v>
       </c>
@@ -3961,54 +3988,55 @@
       <c r="J21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K21" s="23">
+      <c r="K21" s="25"/>
+      <c r="L21" s="23">
         <v>15</v>
       </c>
-      <c r="L21" s="23" t="s">
+      <c r="M21" s="23" t="s">
         <v>357</v>
       </c>
-      <c r="M21" s="20">
+      <c r="N21" s="20">
         <v>1</v>
       </c>
-      <c r="N21" s="20" t="s">
+      <c r="O21" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P21" s="20">
+      <c r="Q21" s="20">
         <v>1</v>
       </c>
-      <c r="Q21" s="20" t="s">
+      <c r="R21" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R21" s="20">
+      <c r="S21" s="20">
         <v>2</v>
       </c>
-      <c r="S21" s="20" t="s">
+      <c r="T21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T21" s="23" t="s">
+      <c r="U21" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="U21" s="23" t="s">
+      <c r="V21" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="V21" s="20">
+      <c r="W21" s="20">
         <v>4</v>
       </c>
-      <c r="W21" s="20" t="s">
+      <c r="X21" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X21" s="20">
+      <c r="Y21" s="20">
         <v>2</v>
       </c>
-      <c r="Y21" s="20" t="s">
+      <c r="Z21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z21" s="23" t="s">
+      <c r="AA21" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC21" s="27"/>
-    </row>
-    <row r="22" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD21" s="27"/>
+    </row>
+    <row r="22" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="23" t="s">
         <v>220</v>
       </c>
@@ -4039,54 +4067,55 @@
       <c r="J22" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K22" s="23">
+      <c r="K22" s="25"/>
+      <c r="L22" s="23">
         <v>15</v>
       </c>
-      <c r="L22" s="23" t="s">
+      <c r="M22" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="M22" s="20">
+      <c r="N22" s="20">
         <v>1</v>
       </c>
-      <c r="N22" s="20" t="s">
+      <c r="O22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P22" s="20">
+      <c r="Q22" s="20">
         <v>1</v>
       </c>
-      <c r="Q22" s="20" t="s">
+      <c r="R22" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R22" s="20">
+      <c r="S22" s="20">
         <v>2</v>
       </c>
-      <c r="S22" s="20" t="s">
+      <c r="T22" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T22" s="23" t="s">
+      <c r="U22" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="U22" s="23" t="s">
+      <c r="V22" s="23" t="s">
         <v>401</v>
       </c>
-      <c r="V22" s="20">
+      <c r="W22" s="20">
         <v>4</v>
       </c>
-      <c r="W22" s="20" t="s">
+      <c r="X22" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X22" s="20">
+      <c r="Y22" s="20">
         <v>2</v>
       </c>
-      <c r="Y22" s="20" t="s">
+      <c r="Z22" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z22" s="23" t="s">
+      <c r="AA22" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC22" s="27"/>
-    </row>
-    <row r="23" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD22" s="27"/>
+    </row>
+    <row r="23" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="23" t="s">
         <v>226</v>
       </c>
@@ -4117,54 +4146,55 @@
       <c r="J23" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K23" s="23">
+      <c r="K23" s="25"/>
+      <c r="L23" s="23">
         <v>15</v>
       </c>
-      <c r="L23" s="23" t="s">
+      <c r="M23" s="23" t="s">
         <v>359</v>
       </c>
-      <c r="M23" s="20">
+      <c r="N23" s="20">
         <v>1</v>
       </c>
-      <c r="N23" s="20" t="s">
+      <c r="O23" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P23" s="20">
+      <c r="Q23" s="20">
         <v>1</v>
       </c>
-      <c r="Q23" s="20" t="s">
+      <c r="R23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R23" s="20">
+      <c r="S23" s="20">
         <v>2</v>
       </c>
-      <c r="S23" s="20" t="s">
+      <c r="T23" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T23" s="23" t="s">
+      <c r="U23" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="U23" s="23" t="s">
+      <c r="V23" s="23" t="s">
         <v>403</v>
       </c>
-      <c r="V23" s="20">
+      <c r="W23" s="20">
         <v>4</v>
       </c>
-      <c r="W23" s="20" t="s">
+      <c r="X23" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X23" s="20">
+      <c r="Y23" s="20">
         <v>2</v>
       </c>
-      <c r="Y23" s="20" t="s">
+      <c r="Z23" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z23" s="23" t="s">
+      <c r="AA23" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC23" s="27"/>
-    </row>
-    <row r="24" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD23" s="27"/>
+    </row>
+    <row r="24" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="23" t="s">
         <v>232</v>
       </c>
@@ -4195,54 +4225,55 @@
       <c r="J24" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K24" s="23">
+      <c r="K24" s="25"/>
+      <c r="L24" s="23">
         <v>15</v>
       </c>
-      <c r="L24" s="23" t="s">
+      <c r="M24" s="23" t="s">
         <v>360</v>
       </c>
-      <c r="M24" s="20">
+      <c r="N24" s="20">
         <v>1</v>
       </c>
-      <c r="N24" s="20" t="s">
+      <c r="O24" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P24" s="20">
+      <c r="Q24" s="20">
         <v>1</v>
       </c>
-      <c r="Q24" s="20" t="s">
+      <c r="R24" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R24" s="20">
+      <c r="S24" s="20">
         <v>2</v>
       </c>
-      <c r="S24" s="20" t="s">
+      <c r="T24" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T24" s="23" t="s">
+      <c r="U24" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="U24" s="23" t="s">
+      <c r="V24" s="23" t="s">
         <v>404</v>
       </c>
-      <c r="V24" s="20">
+      <c r="W24" s="20">
         <v>4</v>
       </c>
-      <c r="W24" s="20" t="s">
+      <c r="X24" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X24" s="20">
+      <c r="Y24" s="20">
         <v>2</v>
       </c>
-      <c r="Y24" s="20" t="s">
+      <c r="Z24" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z24" s="23" t="s">
+      <c r="AA24" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AC24" s="27"/>
-    </row>
-    <row r="25" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD24" s="27"/>
+    </row>
+    <row r="25" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="23" t="s">
         <v>238</v>
       </c>
@@ -4273,54 +4304,55 @@
       <c r="J25" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K25" s="23">
+      <c r="K25" s="25"/>
+      <c r="L25" s="23">
         <v>15</v>
       </c>
-      <c r="L25" s="23" t="s">
+      <c r="M25" s="23" t="s">
         <v>361</v>
       </c>
-      <c r="M25" s="20">
+      <c r="N25" s="20">
         <v>1</v>
       </c>
-      <c r="N25" s="20" t="s">
+      <c r="O25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P25" s="20">
+      <c r="Q25" s="20">
         <v>1</v>
       </c>
-      <c r="Q25" s="20" t="s">
+      <c r="R25" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R25" s="20">
+      <c r="S25" s="20">
         <v>2</v>
       </c>
-      <c r="S25" s="20" t="s">
+      <c r="T25" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T25" s="23" t="s">
+      <c r="U25" s="23" t="s">
         <v>376</v>
       </c>
-      <c r="U25" s="23" t="s">
+      <c r="V25" s="23" t="s">
         <v>405</v>
       </c>
-      <c r="V25" s="20">
+      <c r="W25" s="20">
         <v>4</v>
       </c>
-      <c r="W25" s="20" t="s">
+      <c r="X25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X25" s="20">
+      <c r="Y25" s="20">
         <v>2</v>
       </c>
-      <c r="Y25" s="20" t="s">
+      <c r="Z25" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z25" s="23" t="s">
+      <c r="AA25" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC25" s="27"/>
-    </row>
-    <row r="26" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD25" s="27"/>
+    </row>
+    <row r="26" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="23" t="s">
         <v>244</v>
       </c>
@@ -4351,54 +4383,55 @@
       <c r="J26" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K26" s="23">
+      <c r="K26" s="25"/>
+      <c r="L26" s="23">
         <v>15</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="M26" s="23" t="s">
         <v>362</v>
       </c>
-      <c r="M26" s="20">
+      <c r="N26" s="20">
         <v>1</v>
       </c>
-      <c r="N26" s="20" t="s">
+      <c r="O26" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P26" s="20">
+      <c r="Q26" s="20">
         <v>1</v>
       </c>
-      <c r="Q26" s="20" t="s">
+      <c r="R26" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R26" s="20">
+      <c r="S26" s="20">
         <v>2</v>
       </c>
-      <c r="S26" s="20" t="s">
+      <c r="T26" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T26" s="23" t="s">
+      <c r="U26" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="U26" s="23" t="s">
+      <c r="V26" s="23" t="s">
         <v>388</v>
       </c>
-      <c r="V26" s="20">
+      <c r="W26" s="20">
         <v>4</v>
       </c>
-      <c r="W26" s="20" t="s">
+      <c r="X26" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X26" s="20">
+      <c r="Y26" s="20">
         <v>2</v>
       </c>
-      <c r="Y26" s="20" t="s">
+      <c r="Z26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z26" s="23" t="s">
+      <c r="AA26" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="AC26" s="27"/>
-    </row>
-    <row r="27" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD26" s="27"/>
+    </row>
+    <row r="27" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="23" t="s">
         <v>250</v>
       </c>
@@ -4429,54 +4462,55 @@
       <c r="J27" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K27" s="23">
+      <c r="K27" s="25"/>
+      <c r="L27" s="23">
         <v>15</v>
       </c>
-      <c r="L27" s="23" t="s">
+      <c r="M27" s="23" t="s">
         <v>363</v>
       </c>
-      <c r="M27" s="20">
+      <c r="N27" s="20">
         <v>1</v>
       </c>
-      <c r="N27" s="20" t="s">
+      <c r="O27" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P27" s="20">
+      <c r="Q27" s="20">
         <v>1</v>
       </c>
-      <c r="Q27" s="20" t="s">
+      <c r="R27" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R27" s="20">
+      <c r="S27" s="20">
         <v>2</v>
       </c>
-      <c r="S27" s="20" t="s">
+      <c r="T27" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T27" s="23" t="s">
+      <c r="U27" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="U27" s="23" t="s">
+      <c r="V27" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="V27" s="20">
+      <c r="W27" s="20">
         <v>4</v>
       </c>
-      <c r="W27" s="20" t="s">
+      <c r="X27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X27" s="20">
+      <c r="Y27" s="20">
         <v>2</v>
       </c>
-      <c r="Y27" s="20" t="s">
+      <c r="Z27" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z27" s="23" t="s">
+      <c r="AA27" s="23" t="s">
         <v>419</v>
       </c>
-      <c r="AC27" s="27"/>
-    </row>
-    <row r="28" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD27" s="27"/>
+    </row>
+    <row r="28" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="23" t="s">
         <v>256</v>
       </c>
@@ -4507,54 +4541,55 @@
       <c r="J28" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K28" s="23">
+      <c r="K28" s="25"/>
+      <c r="L28" s="23">
         <v>15</v>
       </c>
-      <c r="L28" s="23" t="s">
+      <c r="M28" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="M28" s="20">
+      <c r="N28" s="20">
         <v>1</v>
       </c>
-      <c r="N28" s="20" t="s">
+      <c r="O28" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P28" s="20">
+      <c r="Q28" s="20">
         <v>1</v>
       </c>
-      <c r="Q28" s="20" t="s">
+      <c r="R28" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R28" s="20">
+      <c r="S28" s="20">
         <v>2</v>
       </c>
-      <c r="S28" s="20" t="s">
+      <c r="T28" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T28" s="23" t="s">
+      <c r="U28" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="U28" s="23" t="s">
+      <c r="V28" s="23" t="s">
         <v>408</v>
       </c>
-      <c r="V28" s="20">
+      <c r="W28" s="20">
         <v>4</v>
       </c>
-      <c r="W28" s="20" t="s">
+      <c r="X28" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X28" s="20">
+      <c r="Y28" s="20">
         <v>2</v>
       </c>
-      <c r="Y28" s="20" t="s">
+      <c r="Z28" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z28" s="23" t="s">
+      <c r="AA28" s="23" t="s">
         <v>418</v>
       </c>
-      <c r="AC28" s="27"/>
-    </row>
-    <row r="29" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD28" s="27"/>
+    </row>
+    <row r="29" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
         <v>262</v>
       </c>
@@ -4585,54 +4620,55 @@
       <c r="J29" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="23">
+      <c r="K29" s="25"/>
+      <c r="L29" s="23">
         <v>15</v>
       </c>
-      <c r="L29" s="23" t="s">
+      <c r="M29" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="M29" s="20">
+      <c r="N29" s="20">
         <v>1</v>
       </c>
-      <c r="N29" s="20" t="s">
+      <c r="O29" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P29" s="20">
+      <c r="Q29" s="20">
         <v>1</v>
       </c>
-      <c r="Q29" s="20" t="s">
+      <c r="R29" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R29" s="20">
+      <c r="S29" s="20">
         <v>2</v>
       </c>
-      <c r="S29" s="20" t="s">
+      <c r="T29" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T29" s="23" t="s">
+      <c r="U29" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="U29" s="23" t="s">
+      <c r="V29" s="23" t="s">
         <v>379</v>
       </c>
-      <c r="V29" s="20">
+      <c r="W29" s="20">
         <v>4</v>
       </c>
-      <c r="W29" s="20" t="s">
+      <c r="X29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X29" s="20">
+      <c r="Y29" s="20">
         <v>2</v>
       </c>
-      <c r="Y29" s="20" t="s">
+      <c r="Z29" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z29" s="23" t="s">
+      <c r="AA29" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC29" s="27"/>
-    </row>
-    <row r="30" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD29" s="27"/>
+    </row>
+    <row r="30" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="23" t="s">
         <v>268</v>
       </c>
@@ -4663,54 +4699,55 @@
       <c r="J30" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K30" s="23">
+      <c r="K30" s="25"/>
+      <c r="L30" s="23">
         <v>15</v>
       </c>
-      <c r="L30" s="23" t="s">
+      <c r="M30" s="23" t="s">
         <v>365</v>
       </c>
-      <c r="M30" s="20">
+      <c r="N30" s="20">
         <v>1</v>
       </c>
-      <c r="N30" s="20" t="s">
+      <c r="O30" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P30" s="20">
+      <c r="Q30" s="20">
         <v>1</v>
       </c>
-      <c r="Q30" s="20" t="s">
+      <c r="R30" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R30" s="20">
+      <c r="S30" s="20">
         <v>2</v>
       </c>
-      <c r="S30" s="20" t="s">
+      <c r="T30" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T30" s="23" t="s">
+      <c r="U30" s="23" t="s">
         <v>387</v>
       </c>
-      <c r="U30" s="23" t="s">
+      <c r="V30" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="V30" s="20">
+      <c r="W30" s="20">
         <v>4</v>
       </c>
-      <c r="W30" s="20" t="s">
+      <c r="X30" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X30" s="20">
+      <c r="Y30" s="20">
         <v>2</v>
       </c>
-      <c r="Y30" s="20" t="s">
+      <c r="Z30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z30" s="23" t="s">
+      <c r="AA30" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AC30" s="27"/>
-    </row>
-    <row r="31" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD30" s="27"/>
+    </row>
+    <row r="31" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="23" t="s">
         <v>274</v>
       </c>
@@ -4741,54 +4778,55 @@
       <c r="J31" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K31" s="23">
+      <c r="K31" s="25"/>
+      <c r="L31" s="23">
         <v>15</v>
       </c>
-      <c r="L31" s="23" t="s">
+      <c r="M31" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="M31" s="20">
+      <c r="N31" s="20">
         <v>1</v>
       </c>
-      <c r="N31" s="20" t="s">
+      <c r="O31" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P31" s="20">
+      <c r="Q31" s="20">
         <v>1</v>
       </c>
-      <c r="Q31" s="20" t="s">
+      <c r="R31" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R31" s="20">
+      <c r="S31" s="20">
         <v>2</v>
       </c>
-      <c r="S31" s="20" t="s">
+      <c r="T31" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T31" s="23" t="s">
+      <c r="U31" s="23" t="s">
         <v>406</v>
       </c>
-      <c r="U31" s="23" t="s">
+      <c r="V31" s="23" t="s">
         <v>410</v>
       </c>
-      <c r="V31" s="20">
+      <c r="W31" s="20">
         <v>4</v>
       </c>
-      <c r="W31" s="20" t="s">
+      <c r="X31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X31" s="20">
+      <c r="Y31" s="20">
         <v>2</v>
       </c>
-      <c r="Y31" s="20" t="s">
+      <c r="Z31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z31" s="23" t="s">
+      <c r="AA31" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AC31" s="27"/>
-    </row>
-    <row r="32" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD31" s="27"/>
+    </row>
+    <row r="32" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23" t="s">
         <v>280</v>
       </c>
@@ -4819,54 +4857,55 @@
       <c r="J32" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K32" s="23">
+      <c r="K32" s="25"/>
+      <c r="L32" s="23">
         <v>15</v>
       </c>
-      <c r="L32" s="23" t="s">
+      <c r="M32" s="23" t="s">
         <v>367</v>
       </c>
-      <c r="M32" s="20">
+      <c r="N32" s="20">
         <v>1</v>
       </c>
-      <c r="N32" s="20" t="s">
+      <c r="O32" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P32" s="20">
+      <c r="Q32" s="20">
         <v>1</v>
       </c>
-      <c r="Q32" s="20" t="s">
+      <c r="R32" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R32" s="20">
+      <c r="S32" s="20">
         <v>2</v>
       </c>
-      <c r="S32" s="20" t="s">
+      <c r="T32" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T32" s="23" t="s">
+      <c r="U32" s="23" t="s">
         <v>381</v>
       </c>
-      <c r="U32" s="23" t="s">
+      <c r="V32" s="23" t="s">
         <v>411</v>
       </c>
-      <c r="V32" s="20">
+      <c r="W32" s="20">
         <v>4</v>
       </c>
-      <c r="W32" s="20" t="s">
+      <c r="X32" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X32" s="20">
+      <c r="Y32" s="20">
         <v>2</v>
       </c>
-      <c r="Y32" s="20" t="s">
+      <c r="Z32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z32" s="23" t="s">
+      <c r="AA32" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="AC32" s="27"/>
-    </row>
-    <row r="33" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD32" s="27"/>
+    </row>
+    <row r="33" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="23" t="s">
         <v>286</v>
       </c>
@@ -4897,54 +4936,55 @@
       <c r="J33" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K33" s="23">
+      <c r="K33" s="25"/>
+      <c r="L33" s="23">
         <v>15</v>
       </c>
-      <c r="L33" s="23" t="s">
+      <c r="M33" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="M33" s="20">
+      <c r="N33" s="20">
         <v>1</v>
       </c>
-      <c r="N33" s="20" t="s">
+      <c r="O33" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P33" s="20">
+      <c r="Q33" s="20">
         <v>1</v>
       </c>
-      <c r="Q33" s="20" t="s">
+      <c r="R33" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R33" s="20">
+      <c r="S33" s="20">
         <v>2</v>
       </c>
-      <c r="S33" s="20" t="s">
+      <c r="T33" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T33" s="23" t="s">
+      <c r="U33" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U33" s="23" t="s">
+      <c r="V33" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="V33" s="20">
+      <c r="W33" s="20">
         <v>4</v>
       </c>
-      <c r="W33" s="20" t="s">
+      <c r="X33" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X33" s="20">
+      <c r="Y33" s="20">
         <v>2</v>
       </c>
-      <c r="Y33" s="20" t="s">
+      <c r="Z33" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z33" s="23" t="s">
+      <c r="AA33" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC33" s="27"/>
-    </row>
-    <row r="34" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD33" s="27"/>
+    </row>
+    <row r="34" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="23" t="s">
         <v>292</v>
       </c>
@@ -4975,54 +5015,55 @@
       <c r="J34" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K34" s="23">
+      <c r="K34" s="25"/>
+      <c r="L34" s="23">
         <v>15</v>
       </c>
-      <c r="L34" s="23" t="s">
+      <c r="M34" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="M34" s="20">
+      <c r="N34" s="20">
         <v>1</v>
       </c>
-      <c r="N34" s="20" t="s">
+      <c r="O34" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P34" s="20">
+      <c r="Q34" s="20">
         <v>1</v>
       </c>
-      <c r="Q34" s="20" t="s">
+      <c r="R34" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R34" s="20">
+      <c r="S34" s="20">
         <v>2</v>
       </c>
-      <c r="S34" s="20" t="s">
+      <c r="T34" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T34" s="23" t="s">
+      <c r="U34" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U34" s="23" t="s">
+      <c r="V34" s="23" t="s">
         <v>409</v>
       </c>
-      <c r="V34" s="20">
+      <c r="W34" s="20">
         <v>4</v>
       </c>
-      <c r="W34" s="20" t="s">
+      <c r="X34" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X34" s="20">
+      <c r="Y34" s="20">
         <v>2</v>
       </c>
-      <c r="Y34" s="20" t="s">
+      <c r="Z34" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z34" s="23" t="s">
+      <c r="AA34" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC34" s="27"/>
-    </row>
-    <row r="35" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD34" s="27"/>
+    </row>
+    <row r="35" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="23" t="s">
         <v>298</v>
       </c>
@@ -5053,54 +5094,55 @@
       <c r="J35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K35" s="23">
+      <c r="K35" s="25"/>
+      <c r="L35" s="23">
         <v>15</v>
       </c>
-      <c r="L35" s="23" t="s">
+      <c r="M35" s="23" t="s">
         <v>369</v>
       </c>
-      <c r="M35" s="20">
+      <c r="N35" s="20">
         <v>1</v>
       </c>
-      <c r="N35" s="20" t="s">
+      <c r="O35" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P35" s="20">
+      <c r="Q35" s="20">
         <v>1</v>
       </c>
-      <c r="Q35" s="20" t="s">
+      <c r="R35" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R35" s="20">
+      <c r="S35" s="20">
         <v>2</v>
       </c>
-      <c r="S35" s="20" t="s">
+      <c r="T35" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T35" s="23" t="s">
+      <c r="U35" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="U35" s="23" t="s">
+      <c r="V35" s="23" t="s">
         <v>413</v>
       </c>
-      <c r="V35" s="20">
+      <c r="W35" s="20">
         <v>4</v>
       </c>
-      <c r="W35" s="20" t="s">
+      <c r="X35" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X35" s="20">
+      <c r="Y35" s="20">
         <v>2</v>
       </c>
-      <c r="Y35" s="20" t="s">
+      <c r="Z35" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z35" s="23" t="s">
+      <c r="AA35" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC35" s="27"/>
-    </row>
-    <row r="36" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD35" s="27"/>
+    </row>
+    <row r="36" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="23" t="s">
         <v>304</v>
       </c>
@@ -5131,53 +5173,54 @@
       <c r="J36" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K36" s="23">
+      <c r="K36" s="25"/>
+      <c r="L36" s="23">
         <v>15</v>
       </c>
-      <c r="L36" s="23" t="s">
+      <c r="M36" s="23" t="s">
         <v>370</v>
       </c>
-      <c r="M36" s="20">
+      <c r="N36" s="20">
         <v>1</v>
       </c>
-      <c r="N36" s="20" t="s">
+      <c r="O36" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P36" s="20">
+      <c r="Q36" s="20">
         <v>1</v>
       </c>
-      <c r="Q36" s="20" t="s">
+      <c r="R36" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R36" s="20">
+      <c r="S36" s="20">
         <v>2</v>
       </c>
-      <c r="S36" s="20" t="s">
+      <c r="T36" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T36" s="23" t="s">
+      <c r="U36" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U36" s="23" t="s">
+      <c r="V36" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="V36" s="20">
+      <c r="W36" s="20">
         <v>4</v>
       </c>
-      <c r="W36" s="20" t="s">
+      <c r="X36" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X36" s="20">
+      <c r="Y36" s="20">
         <v>2</v>
       </c>
-      <c r="Y36" s="20" t="s">
+      <c r="Z36" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z36" s="23" t="s">
+      <c r="AA36" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="37" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="23" t="s">
         <v>309</v>
       </c>
@@ -5208,54 +5251,54 @@
       <c r="J37" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K37" s="23">
+      <c r="L37" s="23">
         <v>14</v>
       </c>
-      <c r="L37" s="23" t="s">
+      <c r="M37" s="23" t="s">
         <v>371</v>
       </c>
-      <c r="M37" s="20">
+      <c r="N37" s="20">
         <v>1</v>
       </c>
-      <c r="N37" s="20" t="s">
+      <c r="O37" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P37" s="20">
+      <c r="Q37" s="20">
         <v>1</v>
       </c>
-      <c r="Q37" s="20" t="s">
+      <c r="R37" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R37" s="20">
+      <c r="S37" s="20">
         <v>2</v>
       </c>
-      <c r="S37" s="20" t="s">
+      <c r="T37" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T37" s="23" t="s">
+      <c r="U37" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U37" s="23" t="s">
+      <c r="V37" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="V37" s="20">
+      <c r="W37" s="20">
         <v>4</v>
       </c>
-      <c r="W37" s="20" t="s">
+      <c r="X37" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X37" s="20">
+      <c r="Y37" s="20">
         <v>2</v>
       </c>
-      <c r="Y37" s="20" t="s">
+      <c r="Z37" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z37" s="23" t="s">
+      <c r="AA37" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="AC37" s="28"/>
-    </row>
-    <row r="38" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD37" s="28"/>
+    </row>
+    <row r="38" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="23" t="s">
         <v>315</v>
       </c>
@@ -5286,53 +5329,53 @@
       <c r="J38" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K38" s="23">
+      <c r="L38" s="23">
         <v>15</v>
       </c>
-      <c r="L38" s="23" t="s">
+      <c r="M38" s="23" t="s">
         <v>372</v>
       </c>
-      <c r="M38" s="20">
+      <c r="N38" s="20">
         <v>1</v>
       </c>
-      <c r="N38" s="20" t="s">
+      <c r="O38" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P38" s="20">
+      <c r="Q38" s="20">
         <v>1</v>
       </c>
-      <c r="Q38" s="20" t="s">
+      <c r="R38" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R38" s="20">
+      <c r="S38" s="20">
         <v>2</v>
       </c>
-      <c r="S38" s="20" t="s">
+      <c r="T38" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T38" s="23" t="s">
+      <c r="U38" s="23" t="s">
         <v>402</v>
       </c>
-      <c r="U38" s="23" t="s">
+      <c r="V38" s="23" t="s">
         <v>407</v>
       </c>
-      <c r="V38" s="20">
+      <c r="W38" s="20">
         <v>4</v>
       </c>
-      <c r="W38" s="20" t="s">
+      <c r="X38" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X38" s="20">
+      <c r="Y38" s="20">
         <v>2</v>
       </c>
-      <c r="Y38" s="20" t="s">
+      <c r="Z38" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z38" s="23" t="s">
+      <c r="AA38" s="23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>321</v>
       </c>
@@ -5363,53 +5406,53 @@
       <c r="J39" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K39" s="23">
+      <c r="L39" s="23">
         <v>15</v>
       </c>
-      <c r="L39" s="23" t="s">
+      <c r="M39" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="M39" s="20">
+      <c r="N39" s="20">
         <v>1</v>
       </c>
-      <c r="N39" s="20" t="s">
+      <c r="O39" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P39" s="20">
+      <c r="Q39" s="20">
         <v>1</v>
       </c>
-      <c r="Q39" s="20" t="s">
+      <c r="R39" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R39" s="20">
+      <c r="S39" s="20">
         <v>2</v>
       </c>
-      <c r="S39" s="20" t="s">
+      <c r="T39" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T39" s="23" t="s">
+      <c r="U39" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U39" s="23" t="s">
+      <c r="V39" s="23" t="s">
         <v>415</v>
       </c>
-      <c r="V39" s="20">
+      <c r="W39" s="20">
         <v>4</v>
       </c>
-      <c r="W39" s="20" t="s">
+      <c r="X39" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X39" s="20">
+      <c r="Y39" s="20">
         <v>2</v>
       </c>
-      <c r="Y39" s="20" t="s">
+      <c r="Z39" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z39" s="23" t="s">
+      <c r="AA39" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>327</v>
       </c>
@@ -5440,53 +5483,53 @@
       <c r="J40" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K40" s="23">
+      <c r="L40" s="23">
         <v>15</v>
       </c>
-      <c r="L40" s="23" t="s">
+      <c r="M40" s="23" t="s">
         <v>374</v>
       </c>
-      <c r="M40" s="20">
+      <c r="N40" s="20">
         <v>1</v>
       </c>
-      <c r="N40" s="20" t="s">
+      <c r="O40" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P40" s="20">
+      <c r="Q40" s="20">
         <v>1</v>
       </c>
-      <c r="Q40" s="20" t="s">
+      <c r="R40" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R40" s="20">
+      <c r="S40" s="20">
         <v>2</v>
       </c>
-      <c r="S40" s="20" t="s">
+      <c r="T40" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T40" s="23" t="s">
+      <c r="U40" s="23" t="s">
         <v>389</v>
       </c>
-      <c r="U40" s="23" t="s">
+      <c r="V40" s="23" t="s">
         <v>413</v>
       </c>
-      <c r="V40" s="20">
+      <c r="W40" s="20">
         <v>4</v>
       </c>
-      <c r="W40" s="20" t="s">
+      <c r="X40" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X40" s="20">
+      <c r="Y40" s="20">
         <v>2</v>
       </c>
-      <c r="Y40" s="20" t="s">
+      <c r="Z40" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z40" s="23" t="s">
+      <c r="AA40" s="23" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="41" spans="1:29" s="20" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="23" t="s">
         <v>332</v>
       </c>
@@ -5517,62 +5560,67 @@
       <c r="J41" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="K41" s="23">
+      <c r="L41" s="23">
         <v>15</v>
       </c>
-      <c r="L41" s="23" t="s">
+      <c r="M41" s="23" t="s">
         <v>373</v>
       </c>
-      <c r="M41" s="20">
+      <c r="N41" s="20">
         <v>1</v>
       </c>
-      <c r="N41" s="20" t="s">
+      <c r="O41" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="P41" s="20">
+      <c r="Q41" s="20">
         <v>1</v>
       </c>
-      <c r="Q41" s="20" t="s">
+      <c r="R41" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="R41" s="20">
+      <c r="S41" s="20">
         <v>2</v>
       </c>
-      <c r="S41" s="20" t="s">
+      <c r="T41" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="T41" s="23" t="s">
+      <c r="U41" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="U41" s="23" t="s">
+      <c r="V41" s="23" t="s">
         <v>417</v>
       </c>
-      <c r="V41" s="20">
+      <c r="W41" s="20">
         <v>4</v>
       </c>
-      <c r="W41" s="20" t="s">
+      <c r="X41" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="X41" s="20">
+      <c r="Y41" s="20">
         <v>2</v>
       </c>
-      <c r="Y41" s="20" t="s">
+      <c r="Z41" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="Z41" s="23" t="s">
+      <c r="AA41" s="23" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="X1:Y1"/>
-    <mergeCell ref="Z1:AA1"/>
+    <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="J1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="W1:X1"/>
   </mergeCells>
+  <conditionalFormatting sqref="K2">
+    <cfRule type="cellIs" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -9745,6 +9793,11 @@
   </sheetData>
   <autoFilter ref="A3:AM43"/>
   <mergeCells count="14">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="O2:T2"/>
     <mergeCell ref="AE2:AF2"/>
     <mergeCell ref="AG2:AH2"/>
     <mergeCell ref="AI2:AJ2"/>
@@ -9754,11 +9807,6 @@
     <mergeCell ref="Y2:Z2"/>
     <mergeCell ref="AA2:AB2"/>
     <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="O2:T2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
   <legacyDrawing r:id="rId1"/>
@@ -9770,11 +9818,11 @@
   <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="H4" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="T13" sqref="T13"/>
+      <selection pane="bottomRight" activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12293,6 +12341,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="C2"/>
+    <mergeCell ref="D2"/>
+    <mergeCell ref="E2"/>
+    <mergeCell ref="F2"/>
+    <mergeCell ref="G2"/>
     <mergeCell ref="M2"/>
     <mergeCell ref="N2"/>
     <mergeCell ref="H2"/>
@@ -12300,11 +12353,6 @@
     <mergeCell ref="J2"/>
     <mergeCell ref="K2"/>
     <mergeCell ref="L2"/>
-    <mergeCell ref="C2"/>
-    <mergeCell ref="D2"/>
-    <mergeCell ref="E2"/>
-    <mergeCell ref="F2"/>
-    <mergeCell ref="G2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>

</xml_diff>